<commit_message>
Remove "fail" records with dictionary and hardcode toxval_type fix
</commit_message>
<xml_diff>
--- a/data/input/calibration_class_dictionary.xlsx
+++ b/data/input/calibration_class_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ToxValDB9\Repo\toxvaldbBMDh\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_59657EC58F79A8D366075C52F37BD2729A4A9642" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01EBD46D-DEFC-4974-A06D-9C32CB0D2356}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FD0639-17AD-4628-97D5-1383899E0EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31290" yWindow="1170" windowWidth="21420" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7771" uniqueCount="1646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7795" uniqueCount="1652">
   <si>
     <t>calibration_string</t>
   </si>
@@ -4961,6 +4961,24 @@
   </si>
   <si>
     <t>BMC</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9020166_BMD (10)_0.03_chronic_18_months</t>
+  </si>
+  <si>
+    <t>BMD (10)</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024305_LOAEL_0.014_-_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID4024305</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4023913_BMD (10)_0.46_chronic_172_weeks</t>
+  </si>
+  <si>
+    <t>172</t>
   </si>
 </sst>
 </file>
@@ -5313,7 +5331,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I978"/>
+  <dimension ref="A1:I981"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -33530,6 +33548,93 @@
         <v>13</v>
       </c>
     </row>
+    <row r="979" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A979" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B979" t="s">
+        <v>394</v>
+      </c>
+      <c r="C979" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D979" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E979">
+        <v>0.03</v>
+      </c>
+      <c r="F979" t="s">
+        <v>27</v>
+      </c>
+      <c r="G979" t="s">
+        <v>286</v>
+      </c>
+      <c r="H979" t="s">
+        <v>36</v>
+      </c>
+      <c r="I979" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="980" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A980" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B980" t="s">
+        <v>394</v>
+      </c>
+      <c r="C980" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D980" t="s">
+        <v>12</v>
+      </c>
+      <c r="E980">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F980" t="s">
+        <v>312</v>
+      </c>
+      <c r="G980" t="s">
+        <v>311</v>
+      </c>
+      <c r="H980" t="s">
+        <v>312</v>
+      </c>
+      <c r="I980" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="981" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A981" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B981" t="s">
+        <v>394</v>
+      </c>
+      <c r="C981" t="s">
+        <v>461</v>
+      </c>
+      <c r="D981" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E981">
+        <v>0.46</v>
+      </c>
+      <c r="F981" t="s">
+        <v>27</v>
+      </c>
+      <c r="G981" t="s">
+        <v>1651</v>
+      </c>
+      <c r="H981" t="s">
+        <v>21</v>
+      </c>
+      <c r="I981" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I978" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated README and select input files
</commit_message>
<xml_diff>
--- a/data/input/calibration_class_dictionary.xlsx
+++ b/data/input/calibration_class_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ToxValDB9\Repo\toxvaldbBMDh\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FD0639-17AD-4628-97D5-1383899E0EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CC9573-C9F3-4C4A-A21D-A66D27E36C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31290" yWindow="1170" windowWidth="21420" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7795" uniqueCount="1652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8827" uniqueCount="1883">
   <si>
     <t>calibration_string</t>
   </si>
@@ -4979,6 +4979,699 @@
   </si>
   <si>
     <t>172</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID4020458_NOAEL_0.1_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID4020458</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID0022018_NOAEL_0.009_chronic_364_days</t>
+  </si>
+  <si>
+    <t>DTXSID0022018</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID0022018_LOAEL_0.06_chronic_2_years</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID1020560_NOAEL_0.7_short-term (developmental)_23_days</t>
+  </si>
+  <si>
+    <t>DTXSID1020560</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID1020560_NOAEL_0.45_chronic_22_weeks</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID1024122_NOAEL_100_short-term (developmental)_13_days</t>
+  </si>
+  <si>
+    <t>DTXSID1024122</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID1024122_NOAEL_113_chronic_24_months</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID3020122_BMDL_1.04_short-term (developmental)_10_days</t>
+  </si>
+  <si>
+    <t>DTXSID3020122</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID3020122_BMDL_0.29_chronic_26_weeks</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID3020122_BMDL_0.3_chronic_52_weeks</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID4020791_NOAEL_0.23_subchronic_56_days</t>
+  </si>
+  <si>
+    <t>DTXSID4020791</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID4020791_NOAEL_2_chronic_2_years</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID1020855_LOAEL_0.22_subchronic_13_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID1020855</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID1020855_NOAEL_0.025_chronic_28_months</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID7021100_NOAEL_0.09_short-term_30_days</t>
+  </si>
+  <si>
+    <t>ATSDR MRLs_DTXSID8022292_NOAEL_15.5_subchronic_13_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID8022292</t>
+  </si>
+  <si>
+    <t>HEAST_DTXSID4020458_NOEL_0.03_short-term_20_days</t>
+  </si>
+  <si>
+    <t>HEAST_DTXSID6032352_NOAEL_1_chronic_3_years</t>
+  </si>
+  <si>
+    <t>DTXSID6032352</t>
+  </si>
+  <si>
+    <t>HEAST_DTXSID0034695_NOEL_2.9_chronic_90_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID0034695</t>
+  </si>
+  <si>
+    <t>HEAST_DTXSID4032459_NOAEL_0.033_subchronic_13_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID4032459</t>
+  </si>
+  <si>
+    <t>HEAST_DTXSID2022254_NOAEL_0.0025_chronic_6_months</t>
+  </si>
+  <si>
+    <t>DTXSID2022254</t>
+  </si>
+  <si>
+    <t>HEAST_DTXSID6032647_NOEL_25_subchronic_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID6032647</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8023848_NOAEL_2_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID8023848</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1022265_NOAEL_1_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID1022265</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6023862_NOAEL_0.11_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID6023862</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9023881_NOEL_1.25_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID9023881</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9020160_NOEL_1.5_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID9020160</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4020242_LEL_2_chronic_1_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1023998_NOEL_1_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID1023998</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0024002_NOAEL_2.5_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID0024002</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024018_NOEL_3_acute (developmental)_1_days</t>
+  </si>
+  <si>
+    <t>DTXSID4024018</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024101_NOEL_0.79_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024101</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024152_NOEL_25_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID3024152</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024154_NOEL_4.2_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID3024154</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024164_NOEL_19.9_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID7024164</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6024177_LEL_0.05_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID6024177</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024238_NOEL_5_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024238</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024280_NOEL_1.25_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024280</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024287_NOEL_25_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID3024287</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024299_NOEL_2.5_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID7024299</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9024304_NOEL_8.86_chronic_1_years</t>
+  </si>
+  <si>
+    <t>DTXSID9024304</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9020370_NOEL_15_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID9020370</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0021387_NOEL_0.75_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8020040_LOAEL_0.025_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6023864_NOEL_25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID6023864</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5023871_NOEL_0.25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID5023871</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3023897_NOEL_2.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID3023897</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5035957_NOEL_2.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID5035957</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3022162_NOEL_5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID3022162</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7021948_LEL_0.36_acute_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID7021948</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3023899_NOAEL_25_chronic_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID3023899</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0023951_NOEL_10_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID0023951</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7023980_NOEL_5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID7023980</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9023914_NOEL_0.1_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID9023914</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0024000_NOAEL_1_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID0024000</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0024052_NOEL_2_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID0024052</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6034554_NOEL_0.22_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0022018_LEL_0.04_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1020560_NOAEL_0.6_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024081_NOEL_2_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID7024081</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6020561_NOEL_0.025_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024102_NOEL_0.025_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID3024102</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1020643_NOEL_250_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1020643</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1024124_NOEL_1.25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1024124</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7020764_NOEL_50_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID7020764</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID2023981_NOAEL (ADJ)_1468_chronic_-999_-</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024151_NOEL_1.25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024151</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024159_NOEL_5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024159</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5020819_NOEL_0.1_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID5020819</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1022267_NOEL_2.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1022267</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1020855_NOEL_0.025_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4022448_NOEL_15_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID4022448</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6024204_NOEL_2.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID6024204</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1024209_NOEL_0.2_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1024209</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024239_NOEL_0.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID3024239</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6021086_NOEL_2.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID6021086</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024245_NOEL_12.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID7024245</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8022292_NOEL_5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1024255_NOAEL_25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1024255</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5024261_NOEL_2_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID5024261</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID2020420_NOEL_7.5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID2020420</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8022111_NOEL_5_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID8022111</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024315_NOEL_2.49_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024315</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024317_NOEL_1.25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID8024317</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024318_NOEL_0.1_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID3024318</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6024337_NOEL_1_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID6024337</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1024338_NOEL_8_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1024338</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0024343_NOEL_0.75_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID0024343</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5024344_NOAEL_1.275_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID5024344</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0024345_NOEL_1.2_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID0024345</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5021465_LOAEL_25_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID5021465</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024328_NOEL_0.5_subchronic_3_months</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6023999_NOEL_0.75_chronic_6_months</t>
+  </si>
+  <si>
+    <t>DTXSID6023999</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6024175_NOEL_6.25_chronic_6_months</t>
+  </si>
+  <si>
+    <t>DTXSID6024175</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024234_NOEL_3.75_chronic_6_months</t>
+  </si>
+  <si>
+    <t>DTXSID8024234</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4022361_NOEL_2.5_chronic_6_months</t>
+  </si>
+  <si>
+    <t>DTXSID4022361</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024108_NOEL_1.8_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID3024108</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4021395_NOEL_0.75_chronic_12_months</t>
+  </si>
+  <si>
+    <t>DTXSID4021395</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024193_NOEL_12_subchronic_13_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID4024193</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1023869_NOEL_8.6_subchronic_13_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID1023869</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1024122_NOEL_10_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID1024120_NOEL_0.4_subchronic_13_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID1024120</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID9020827_NOEL_5.01_short-term (developmental)_13_days</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024276_NOEL_2_short-term (developmental)_13_days</t>
+  </si>
+  <si>
+    <t>DTXSID4024276</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6024252_NOEL_0.007_short-term_14_days</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024085_LEL_0.5_short-term_16_days</t>
+  </si>
+  <si>
+    <t>DTXSID7024085</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6024206_NOEL_0.2_-_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID6024206</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024241_NOEL_0.3_chronic_20_months</t>
+  </si>
+  <si>
+    <t>DTXSID7024241</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID2024086_NOEL_0.05_short-term_21_days</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID5024211_NOEL_30_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID5024211</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6023868_NOEL_0.33_chronic_26_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID6023868</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4020791_NOEL_0.23_subchronic_47_days</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID0024266_NOEL_0.25_subchronic_56_days</t>
+  </si>
+  <si>
+    <t>DTXSID0024266</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024160_LEL_1.5_chronic_78_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID7024160</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7024035_NOAEL_8_subchronic_90_days</t>
+  </si>
+  <si>
+    <t>DTXSID7024035</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024193_NOEL_12_subchronic_90_days</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8023846_LEL_0.12_subchronic_90_days</t>
+  </si>
+  <si>
+    <t>DTXSID8023846</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID6021248_NOEL_0.38_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID6021248</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID2024242_NOEL_12.5_subchronic_90_days</t>
+  </si>
+  <si>
+    <t>DTXSID2024242</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024274_NOEL_13.3_subchronic_90_days</t>
+  </si>
+  <si>
+    <t>DTXSID4024274</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID3024316_NOEL_7_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID3024316</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7020895_NOAEL_0.07_chronic_104_weeks</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID4024272_NOEL_3.75_chronic_106_weeks</t>
+  </si>
+  <si>
+    <t>DTXSID4024272</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>PPRTV (CPHEA)_DTXSID1040320_LOAEL_7_chronic_2_years</t>
+  </si>
+  <si>
+    <t>DTXSID1040320</t>
+  </si>
+  <si>
+    <t>PPRTV (CPHEA)_DTXSID1040320_NOAEL_145_chronic_52_weeks</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8023890_LEL_50_-_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID8023890</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID8024109_LEL_63.7_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID8024109</t>
+  </si>
+  <si>
+    <t>IRIS_DTXSID7022253_LEL_25_chronic (developmental)_-999_-</t>
+  </si>
+  <si>
+    <t>DTXSID7022253</t>
   </si>
 </sst>
 </file>
@@ -5331,9 +6024,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I981"/>
+  <dimension ref="A1:I1110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1081" workbookViewId="0">
+      <selection activeCell="A1106" sqref="A1106"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33635,6 +34330,3747 @@
         <v>27</v>
       </c>
     </row>
+    <row r="982" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B982" t="s">
+        <v>10</v>
+      </c>
+      <c r="C982" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D982" t="s">
+        <v>32</v>
+      </c>
+      <c r="E982">
+        <v>0.1</v>
+      </c>
+      <c r="F982" t="s">
+        <v>27</v>
+      </c>
+      <c r="G982" t="s">
+        <v>28</v>
+      </c>
+      <c r="H982" t="s">
+        <v>29</v>
+      </c>
+      <c r="I982" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="983" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B983" t="s">
+        <v>10</v>
+      </c>
+      <c r="C983" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D983" t="s">
+        <v>32</v>
+      </c>
+      <c r="E983">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F983" t="s">
+        <v>27</v>
+      </c>
+      <c r="G983" t="s">
+        <v>33</v>
+      </c>
+      <c r="H983" t="s">
+        <v>15</v>
+      </c>
+      <c r="I983" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="984" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A984" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B984" t="s">
+        <v>10</v>
+      </c>
+      <c r="C984" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D984" t="s">
+        <v>12</v>
+      </c>
+      <c r="E984">
+        <v>0.06</v>
+      </c>
+      <c r="F984" t="s">
+        <v>27</v>
+      </c>
+      <c r="G984" t="s">
+        <v>28</v>
+      </c>
+      <c r="H984" t="s">
+        <v>29</v>
+      </c>
+      <c r="I984" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="985" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A985" t="s">
+        <v>1657</v>
+      </c>
+      <c r="B985" t="s">
+        <v>10</v>
+      </c>
+      <c r="C985" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D985" t="s">
+        <v>32</v>
+      </c>
+      <c r="E985">
+        <v>0.7</v>
+      </c>
+      <c r="F985" t="s">
+        <v>51</v>
+      </c>
+      <c r="G985" t="s">
+        <v>848</v>
+      </c>
+      <c r="H985" t="s">
+        <v>15</v>
+      </c>
+      <c r="I985" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="986" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B986" t="s">
+        <v>10</v>
+      </c>
+      <c r="C986" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D986" t="s">
+        <v>32</v>
+      </c>
+      <c r="E986">
+        <v>0.45</v>
+      </c>
+      <c r="F986" t="s">
+        <v>27</v>
+      </c>
+      <c r="G986" t="s">
+        <v>860</v>
+      </c>
+      <c r="H986" t="s">
+        <v>21</v>
+      </c>
+      <c r="I986" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="987" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B987" t="s">
+        <v>10</v>
+      </c>
+      <c r="C987" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D987" t="s">
+        <v>32</v>
+      </c>
+      <c r="E987">
+        <v>100</v>
+      </c>
+      <c r="F987" t="s">
+        <v>51</v>
+      </c>
+      <c r="G987" t="s">
+        <v>20</v>
+      </c>
+      <c r="H987" t="s">
+        <v>15</v>
+      </c>
+      <c r="I987" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="988" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B988" t="s">
+        <v>10</v>
+      </c>
+      <c r="C988" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D988" t="s">
+        <v>32</v>
+      </c>
+      <c r="E988">
+        <v>113</v>
+      </c>
+      <c r="F988" t="s">
+        <v>27</v>
+      </c>
+      <c r="G988" t="s">
+        <v>35</v>
+      </c>
+      <c r="H988" t="s">
+        <v>36</v>
+      </c>
+      <c r="I988" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="989" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A989" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B989" t="s">
+        <v>10</v>
+      </c>
+      <c r="C989" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D989" t="s">
+        <v>32</v>
+      </c>
+      <c r="E989">
+        <v>113</v>
+      </c>
+      <c r="F989" t="s">
+        <v>27</v>
+      </c>
+      <c r="G989" t="s">
+        <v>35</v>
+      </c>
+      <c r="H989" t="s">
+        <v>36</v>
+      </c>
+      <c r="I989" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="990" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A990" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B990" t="s">
+        <v>10</v>
+      </c>
+      <c r="C990" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D990" t="s">
+        <v>126</v>
+      </c>
+      <c r="E990">
+        <v>1.04</v>
+      </c>
+      <c r="F990" t="s">
+        <v>51</v>
+      </c>
+      <c r="G990" t="s">
+        <v>255</v>
+      </c>
+      <c r="H990" t="s">
+        <v>15</v>
+      </c>
+      <c r="I990" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="991" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A991" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B991" t="s">
+        <v>10</v>
+      </c>
+      <c r="C991" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D991" t="s">
+        <v>126</v>
+      </c>
+      <c r="E991">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F991" t="s">
+        <v>27</v>
+      </c>
+      <c r="G991" t="s">
+        <v>90</v>
+      </c>
+      <c r="H991" t="s">
+        <v>21</v>
+      </c>
+      <c r="I991" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="992" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A992" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B992" t="s">
+        <v>10</v>
+      </c>
+      <c r="C992" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D992" t="s">
+        <v>126</v>
+      </c>
+      <c r="E992">
+        <v>0.3</v>
+      </c>
+      <c r="F992" t="s">
+        <v>27</v>
+      </c>
+      <c r="G992" t="s">
+        <v>1241</v>
+      </c>
+      <c r="H992" t="s">
+        <v>21</v>
+      </c>
+      <c r="I992" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="993" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A993" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B993" t="s">
+        <v>10</v>
+      </c>
+      <c r="C993" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D993" t="s">
+        <v>32</v>
+      </c>
+      <c r="E993">
+        <v>0.23</v>
+      </c>
+      <c r="F993" t="s">
+        <v>13</v>
+      </c>
+      <c r="G993" t="s">
+        <v>1669</v>
+      </c>
+      <c r="H993" t="s">
+        <v>15</v>
+      </c>
+      <c r="I993" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="994" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A994" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B994" t="s">
+        <v>10</v>
+      </c>
+      <c r="C994" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D994" t="s">
+        <v>32</v>
+      </c>
+      <c r="E994">
+        <v>2</v>
+      </c>
+      <c r="F994" t="s">
+        <v>27</v>
+      </c>
+      <c r="G994" t="s">
+        <v>28</v>
+      </c>
+      <c r="H994" t="s">
+        <v>29</v>
+      </c>
+      <c r="I994" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="995" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A995" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B995" t="s">
+        <v>10</v>
+      </c>
+      <c r="C995" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D995" t="s">
+        <v>12</v>
+      </c>
+      <c r="E995">
+        <v>0.22</v>
+      </c>
+      <c r="F995" t="s">
+        <v>13</v>
+      </c>
+      <c r="G995" t="s">
+        <v>20</v>
+      </c>
+      <c r="H995" t="s">
+        <v>21</v>
+      </c>
+      <c r="I995" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="996" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A996" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B996" t="s">
+        <v>10</v>
+      </c>
+      <c r="C996" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D996" t="s">
+        <v>32</v>
+      </c>
+      <c r="E996">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F996" t="s">
+        <v>27</v>
+      </c>
+      <c r="G996" t="s">
+        <v>157</v>
+      </c>
+      <c r="H996" t="s">
+        <v>36</v>
+      </c>
+      <c r="I996" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A997" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B997" t="s">
+        <v>10</v>
+      </c>
+      <c r="C997" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D997" t="s">
+        <v>32</v>
+      </c>
+      <c r="E997">
+        <v>0.09</v>
+      </c>
+      <c r="F997" t="s">
+        <v>41</v>
+      </c>
+      <c r="G997" t="s">
+        <v>70</v>
+      </c>
+      <c r="H997" t="s">
+        <v>15</v>
+      </c>
+      <c r="I997" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="998" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A998" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B998" t="s">
+        <v>10</v>
+      </c>
+      <c r="C998" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D998" t="s">
+        <v>32</v>
+      </c>
+      <c r="E998">
+        <v>15.5</v>
+      </c>
+      <c r="F998" t="s">
+        <v>13</v>
+      </c>
+      <c r="G998" t="s">
+        <v>20</v>
+      </c>
+      <c r="H998" t="s">
+        <v>21</v>
+      </c>
+      <c r="I998" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="999" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A999" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B999" t="s">
+        <v>370</v>
+      </c>
+      <c r="C999" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D999" t="s">
+        <v>210</v>
+      </c>
+      <c r="E999">
+        <v>0.03</v>
+      </c>
+      <c r="F999" t="s">
+        <v>41</v>
+      </c>
+      <c r="G999" t="s">
+        <v>53</v>
+      </c>
+      <c r="H999" t="s">
+        <v>15</v>
+      </c>
+      <c r="I999" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1000" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>1679</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1000">
+        <v>1</v>
+      </c>
+      <c r="F1000" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1000" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1000" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1000" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1001" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1001">
+        <v>2.9</v>
+      </c>
+      <c r="F1001" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1001" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1001" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1001" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1002" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1002">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F1002" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1002" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1002" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1002" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1003" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1003">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1003" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1003" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1004" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1004">
+        <v>25</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1004" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1004" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1004" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1005" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1005">
+        <v>2</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1005" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1005" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1005" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1006" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1006">
+        <v>1</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1006" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1006" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1006" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1007" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1007">
+        <v>0.11</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1007" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1007" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1007" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1008" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1008">
+        <v>1.25</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1008" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1008" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1008" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1009" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1009">
+        <v>1.5</v>
+      </c>
+      <c r="F1009" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1009" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1009" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1009" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1010" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1010">
+        <v>2</v>
+      </c>
+      <c r="F1010" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1010" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1010" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1010" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1011" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1011">
+        <v>1</v>
+      </c>
+      <c r="F1011" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1011" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1011" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1011" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1012" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1012">
+        <v>2.5</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1012" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1012" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1012" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1013" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1013">
+        <v>3</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G1013" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1013" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1013" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1014" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D1014" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1014">
+        <v>0.79</v>
+      </c>
+      <c r="F1014" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1014" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1014" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1014" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1015" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>1708</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1015">
+        <v>25</v>
+      </c>
+      <c r="F1015" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1015" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1015" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1015" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1016" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D1016" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1016">
+        <v>4.2</v>
+      </c>
+      <c r="F1016" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1016" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1016" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1016" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1017" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1017">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F1017" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1017" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1017" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1017" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1018" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1018">
+        <v>0.05</v>
+      </c>
+      <c r="F1018" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1018" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1018" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1018" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1019" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1019">
+        <v>5</v>
+      </c>
+      <c r="F1019" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1019" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1019" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1019" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1020" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1020">
+        <v>1.25</v>
+      </c>
+      <c r="F1020" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1020" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1020" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1020" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1021" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>1720</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1021">
+        <v>25</v>
+      </c>
+      <c r="F1021" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1021" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1021" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1021" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1022" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>1722</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1022">
+        <v>2.5</v>
+      </c>
+      <c r="F1022" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1022" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1022" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1022" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1023" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1023">
+        <v>8.86</v>
+      </c>
+      <c r="F1023" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1023" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1023" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1023" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1024" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1024">
+        <v>15</v>
+      </c>
+      <c r="F1024" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1024" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1024" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1024" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1025" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1025">
+        <v>0.75</v>
+      </c>
+      <c r="F1025" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1025" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1025" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1025" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1026" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>972</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1026">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F1026" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1026" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1026" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1026" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1027" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>1730</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1027">
+        <v>25</v>
+      </c>
+      <c r="F1027" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1027" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1027" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1027" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1028" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D1028" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1028">
+        <v>0.25</v>
+      </c>
+      <c r="F1028" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1028" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1028" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1028" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1029" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D1029" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1029">
+        <v>2.5</v>
+      </c>
+      <c r="F1029" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1029" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1029" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1029" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1030" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>1736</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1030">
+        <v>2.5</v>
+      </c>
+      <c r="F1030" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1030" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1030" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1030" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1031" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>1738</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1031">
+        <v>5</v>
+      </c>
+      <c r="F1031" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1031" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1031" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1031" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1032" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1032" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1032">
+        <v>0.36</v>
+      </c>
+      <c r="F1032" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1032" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1032" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1032" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1033" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D1033" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1033">
+        <v>25</v>
+      </c>
+      <c r="F1033" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1033" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1033" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1033" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1034" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1034">
+        <v>10</v>
+      </c>
+      <c r="F1034" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1034" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1034" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1034" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1035" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D1035" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1035">
+        <v>5</v>
+      </c>
+      <c r="F1035" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1035" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1035" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1035" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1036" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D1036" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1036">
+        <v>0.1</v>
+      </c>
+      <c r="F1036" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1036" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1036" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1036" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1037" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D1037" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1037">
+        <v>1</v>
+      </c>
+      <c r="F1037" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1037" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1037" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1037" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1038" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1038">
+        <v>2</v>
+      </c>
+      <c r="F1038" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1038" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1038" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1038" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1039" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1039">
+        <v>0.22</v>
+      </c>
+      <c r="F1039" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1039" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1039" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1039" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1040" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1040">
+        <v>0.04</v>
+      </c>
+      <c r="F1040" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1040" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1040" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1040" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1041" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1041">
+        <v>0.6</v>
+      </c>
+      <c r="F1041" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1041" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1041" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1041" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1042" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1042">
+        <v>2</v>
+      </c>
+      <c r="F1042" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1042" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1042" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1042" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1043" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1043">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F1043" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1043" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1043" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1043" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1044" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1044">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F1044" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1044" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1044" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1044" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1045" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1045">
+        <v>250</v>
+      </c>
+      <c r="F1045" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1045" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1045" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1045" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1046" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1046">
+        <v>1.25</v>
+      </c>
+      <c r="F1046" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1046" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1046" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1046" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1047" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1047">
+        <v>50</v>
+      </c>
+      <c r="F1047" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1047" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1047" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1047" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1048" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>492</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>325</v>
+      </c>
+      <c r="E1048">
+        <v>1468</v>
+      </c>
+      <c r="F1048" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1048" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1048" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1048" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1049" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1049">
+        <v>1.25</v>
+      </c>
+      <c r="F1049" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1049" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1049" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1049" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1050" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1050">
+        <v>5</v>
+      </c>
+      <c r="F1050" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1050" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1050" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1050" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1051" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1051">
+        <v>0.1</v>
+      </c>
+      <c r="F1051" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1051" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1051" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1051" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1052" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1052">
+        <v>2.5</v>
+      </c>
+      <c r="F1052" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1052" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1052" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1052" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1053" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1053">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F1053" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1053" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1053" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1053" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1054" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>1778</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1054">
+        <v>15</v>
+      </c>
+      <c r="F1054" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1054" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1054" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1054" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1055" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1055">
+        <v>2.5</v>
+      </c>
+      <c r="F1055" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1055" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1055" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1055" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1056" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>1782</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1056">
+        <v>0.2</v>
+      </c>
+      <c r="F1056" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1056" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1056" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1056" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1057" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1057">
+        <v>0.5</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1057" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1057" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1057" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1058" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>1786</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1058">
+        <v>2.5</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1058" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1058" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1058" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1059" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>1788</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1059">
+        <v>12.5</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1059" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1059" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1059" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1060" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1060">
+        <v>5</v>
+      </c>
+      <c r="F1060" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1060" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1060" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1060" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1061" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>1791</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1061">
+        <v>25</v>
+      </c>
+      <c r="F1061" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1061" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1061" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1061" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1062" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1062">
+        <v>2</v>
+      </c>
+      <c r="F1062" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1062" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1062" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1062" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1063" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>1795</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1063">
+        <v>7.5</v>
+      </c>
+      <c r="F1063" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1063" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1063" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1063" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1064" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1064">
+        <v>5</v>
+      </c>
+      <c r="F1064" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1064" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1064" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1064" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1065" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1065">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="F1065" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1065" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1065" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1065" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1066" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>1801</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1066">
+        <v>1.25</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1066" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1066" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1066" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1067" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1067">
+        <v>0.1</v>
+      </c>
+      <c r="F1067" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1067" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1067" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1067" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1068" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1068">
+        <v>1</v>
+      </c>
+      <c r="F1068" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1068" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1068" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1068" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1069" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1069">
+        <v>8</v>
+      </c>
+      <c r="F1069" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1069" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1069" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1069" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1070" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1070">
+        <v>0.75</v>
+      </c>
+      <c r="F1070" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1070" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1070" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1070" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1071" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>1811</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1071">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="F1071" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1071" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1071" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1071" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1072" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>1813</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1072">
+        <v>1.2</v>
+      </c>
+      <c r="F1072" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1072" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1072" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1072" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1073" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1073">
+        <v>25</v>
+      </c>
+      <c r="F1073" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1073" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1073" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1073" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1074" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1074">
+        <v>0.5</v>
+      </c>
+      <c r="F1074" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1074" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1074" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1074" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1075" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1075">
+        <v>0.75</v>
+      </c>
+      <c r="F1075" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1075" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1075" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1075" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1076" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1076">
+        <v>6.25</v>
+      </c>
+      <c r="F1076" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1076" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1076" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1076" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1077" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>1822</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1077">
+        <v>3.75</v>
+      </c>
+      <c r="F1077" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1077" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1077" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1077" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1078" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1078">
+        <v>2.5</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1078" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1078" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1078" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1079" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1079">
+        <v>1.8</v>
+      </c>
+      <c r="F1079" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1079" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1079" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1079" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1080" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1080">
+        <v>0.75</v>
+      </c>
+      <c r="F1080" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1080" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1080" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1080" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1081" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1081">
+        <v>12</v>
+      </c>
+      <c r="F1081" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1081" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1081" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1081" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1082" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>1832</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1082">
+        <v>8.6</v>
+      </c>
+      <c r="F1082" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1082" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1082" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1082" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1083" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1083">
+        <v>10</v>
+      </c>
+      <c r="F1083" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1083" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1083" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1083" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1084" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1084">
+        <v>0.4</v>
+      </c>
+      <c r="F1084" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1084" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1084" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1084" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1085" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1085">
+        <v>5.01</v>
+      </c>
+      <c r="F1085" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1085" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1085" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1085" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1086" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1086">
+        <v>2</v>
+      </c>
+      <c r="F1086" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1086" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1086" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1086" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1087" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>582</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1087">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F1087" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1087" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1087" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1087" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1088" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1088">
+        <v>0.5</v>
+      </c>
+      <c r="F1088" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1088" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1088" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1088" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1089" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1089">
+        <v>0.2</v>
+      </c>
+      <c r="F1089" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1089" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1089" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1089" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1090" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1090">
+        <v>0.3</v>
+      </c>
+      <c r="F1090" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1090" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1090" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1090" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1091" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1091">
+        <v>0.05</v>
+      </c>
+      <c r="F1091" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1091" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1091" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1091" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1092" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1092">
+        <v>30</v>
+      </c>
+      <c r="F1092" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1092" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1092" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1092" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1093" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>1850</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1093">
+        <v>0.33</v>
+      </c>
+      <c r="F1093" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1093" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1093" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1093" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1094" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1094">
+        <v>0.23</v>
+      </c>
+      <c r="F1094" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1094" t="s">
+        <v>1852</v>
+      </c>
+      <c r="H1094" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1094" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1095" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1095">
+        <v>0.25</v>
+      </c>
+      <c r="F1095" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1095" t="s">
+        <v>1669</v>
+      </c>
+      <c r="H1095" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1095" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1096" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1096">
+        <v>1.5</v>
+      </c>
+      <c r="F1096" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1096" t="s">
+        <v>716</v>
+      </c>
+      <c r="H1096" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1096" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1097" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>1858</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1097">
+        <v>8</v>
+      </c>
+      <c r="F1097" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1097" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1097" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1097" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1098" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1098">
+        <v>12</v>
+      </c>
+      <c r="F1098" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1098" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1098" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1098" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1099" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>1861</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1099">
+        <v>0.12</v>
+      </c>
+      <c r="F1099" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1099" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1099" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1099" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1100" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>1863</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1100">
+        <v>0.38</v>
+      </c>
+      <c r="F1100" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1100" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1100" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1100" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1101" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>1865</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1101">
+        <v>12.5</v>
+      </c>
+      <c r="F1101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1101" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1102" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>1867</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1102">
+        <v>13.3</v>
+      </c>
+      <c r="F1102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1102" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1102" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1102" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1103" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1103">
+        <v>7</v>
+      </c>
+      <c r="F1103" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1103" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1103" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1103" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1104" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1104">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F1104" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1104" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1104" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1104" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1105" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>1872</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1105">
+        <v>3.75</v>
+      </c>
+      <c r="F1105" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1105" t="s">
+        <v>1873</v>
+      </c>
+      <c r="H1105" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1105" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1106" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>1875</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1106">
+        <v>7</v>
+      </c>
+      <c r="F1106" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1106" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1106" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1106" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1107" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>1875</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1107">
+        <v>145</v>
+      </c>
+      <c r="F1107" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1107" t="s">
+        <v>1241</v>
+      </c>
+      <c r="H1107" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1108" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>1878</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1108">
+        <v>50</v>
+      </c>
+      <c r="F1108" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1108" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1108" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1108" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1109" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>1880</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1109">
+        <v>63.7</v>
+      </c>
+      <c r="F1109" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1109" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1109" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1109" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1110" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>1882</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1110">
+        <v>25</v>
+      </c>
+      <c r="F1110" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1110" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1110" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1110" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I978" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>